<commit_message>
updated stuff and folder
</commit_message>
<xml_diff>
--- a/T5.1/MSLR/OLD/Coding copy.xlsx
+++ b/T5.1/MSLR/OLD/Coding copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bellerofonte/Dropbox/anita/T5.1/MSLR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bellerofonte/Dropbox/anita/T5.1/MSLR/OLD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2B10A8-47AC-DD46-9C8F-A37FA34645AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02E0677-DD42-8F40-912C-3A2A1747D13F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" activeTab="7" xr2:uid="{2CA368CD-C47B-0B47-AEA0-2A188F39C3E5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" activeTab="6" xr2:uid="{2CA368CD-C47B-0B47-AEA0-2A188F39C3E5}"/>
   </bookViews>
   <sheets>
     <sheet name="CodesInstances - Pilot + Exp" sheetId="1" r:id="rId1"/>
@@ -1844,7 +1844,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1979,6 +1979,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2073,31 +2076,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35</c:v>
+                  <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>59</c:v>
+                  <c:v>590</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5257,7 +5260,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6876,8 +6879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB4DAB1-742F-1F46-B704-DFC97CFEEA89}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7097,17 +7100,17 @@
       </c>
     </row>
     <row r="27" spans="2:4">
-      <c r="B27" s="34" t="s">
+      <c r="C27" s="34"/>
+    </row>
+    <row r="28" spans="2:4" ht="17">
+      <c r="B28" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="C27" s="34"/>
-    </row>
-    <row r="28" spans="2:4" ht="17">
       <c r="C28" s="64" t="s">
         <v>262</v>
       </c>
       <c r="D28">
-        <v>9</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="17">
@@ -7115,7 +7118,7 @@
         <v>261</v>
       </c>
       <c r="D29">
-        <v>35</v>
+        <v>350</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="17">
@@ -7123,7 +7126,7 @@
         <v>260</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="17">
@@ -7131,7 +7134,7 @@
         <v>259</v>
       </c>
       <c r="D31">
-        <v>22</v>
+        <v>220</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="17">
@@ -7139,42 +7142,42 @@
         <v>251</v>
       </c>
       <c r="D32">
-        <v>9</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="17">
-      <c r="C33" s="64" t="s">
+      <c r="B33" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="C33" s="66" t="s">
         <v>258</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="17">
-      <c r="B34" s="34" t="s">
-        <v>256</v>
-      </c>
-      <c r="C34" s="64" t="s">
+      <c r="C34" s="66" t="s">
         <v>249</v>
       </c>
       <c r="D34">
-        <v>7</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="17">
-      <c r="C35" s="64" t="s">
+      <c r="C35" s="66" t="s">
         <v>257</v>
       </c>
       <c r="D35">
-        <v>59</v>
+        <v>590</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="17">
-      <c r="C36" s="64" t="s">
+      <c r="C36" s="66" t="s">
         <v>253</v>
       </c>
       <c r="D36">
-        <v>10</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -7342,8 +7345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7BF439D-8DC3-D041-B8DB-31E5DB138FE7}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7841,8 +7844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C89A6A-E8A8-E445-9BBD-7E973BD63ED7}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7967,7 +7970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5F049E-A6C5-5244-BF20-A4839B0CE8BD}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
committed mod to dataset
</commit_message>
<xml_diff>
--- a/T5.1/MSLR/OLD/Coding copy.xlsx
+++ b/T5.1/MSLR/OLD/Coding copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bellerofonte/Dropbox/anita/T5.1/MSLR/OLD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02E0677-DD42-8F40-912C-3A2A1747D13F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED4258F-79A0-3949-9AE0-C57C24702355}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" activeTab="6" xr2:uid="{2CA368CD-C47B-0B47-AEA0-2A188F39C3E5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" activeTab="8" xr2:uid="{2CA368CD-C47B-0B47-AEA0-2A188F39C3E5}"/>
   </bookViews>
   <sheets>
     <sheet name="CodesInstances - Pilot + Exp" sheetId="1" r:id="rId1"/>
@@ -7191,7 +7191,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7338,6 +7338,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -7844,8 +7845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C89A6A-E8A8-E445-9BBD-7E973BD63ED7}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7970,8 +7971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5F049E-A6C5-5244-BF20-A4839B0CE8BD}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8310,6 +8311,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -8317,8 +8319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C444E0B-31FB-F247-BE78-B0ED671C3305}">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9125,6 +9127,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>